<commit_message>
add label moving sheets
</commit_message>
<xml_diff>
--- a/formatted_cavern/swap_positronic.xlsx
+++ b/formatted_cavern/swap_positronic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afern\Documents\UMD\LHCb\cern\LV_cavern_mapping\formatted_cavern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5705626-ED73-44CD-B0D0-8273F963038C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE73646-BA49-4B97-A7AA-97F94989F166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10190" yWindow="11430" windowWidth="16200" windowHeight="10200" xr2:uid="{5E8DA185-E4B2-4A1D-8A8F-4431A6A6897D}"/>
+    <workbookView xWindow="-10300" yWindow="11320" windowWidth="19420" windowHeight="10420" xr2:uid="{5E8DA185-E4B2-4A1D-8A8F-4431A6A6897D}"/>
   </bookViews>
   <sheets>
     <sheet name="swap" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Positronic</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Pins Match</t>
+  </si>
+  <si>
+    <t>Note: the user should also be careful that the swapped Positronics have the SAME PINS (not just total number) populated</t>
   </si>
 </sst>
 </file>
@@ -446,23 +449,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB3A21A-B25E-4A64-A233-E018DB0155ED}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="4"/>
-    <col min="5" max="5" width="15.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="4"/>
+    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -481,8 +484,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -493,7 +497,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="str">
         <f>IF(ISERROR(VLOOKUP($A2,$D$1:$D$25,1,FALSE)),"No","Yes")</f>
@@ -503,8 +507,11 @@
         <f>IF($B2=LOOKUP($D2,$A$2:$A$25,$C$2:$C$25), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -526,7 +533,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -548,7 +555,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -570,7 +577,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -592,7 +599,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -614,7 +621,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -636,7 +643,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -658,7 +665,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -669,7 +676,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -680,7 +687,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -702,7 +709,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -724,7 +731,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -746,7 +753,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -768,7 +775,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -790,7 +797,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -812,7 +819,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -834,7 +841,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -856,7 +863,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -878,7 +885,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -900,7 +907,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>22</v>
       </c>
@@ -922,7 +929,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>25</v>
       </c>
@@ -944,7 +951,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>28</v>
       </c>
@@ -966,7 +973,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>31</v>
       </c>
@@ -988,7 +995,7 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>34</v>
       </c>

</xml_diff>